<commit_message>
Update to data, bokeh and option initialization.
</commit_message>
<xml_diff>
--- a/examples/data_input/data_structure.xlsx
+++ b/examples/data_input/data_structure.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riw\Documents\pomato\examples\data_input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riw\tubCloud\Uni\Market_Tool\pomato_studies\data_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDB3B55-25CB-4C0B-B8F5-CF5CC7FDF9E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{392C7022-03AC-472B-83F6-72FAC9E760B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2844" yWindow="0" windowWidth="26892" windowHeight="17280" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="948" yWindow="0" windowWidth="26892" windowHeight="17280" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="7" r:id="rId1"/>
     <sheet name="ramses" sheetId="5" r:id="rId2"/>
     <sheet name="opsd" sheetId="8" r:id="rId3"/>
     <sheet name="ieee" sheetId="6" r:id="rId4"/>
+    <sheet name="nrel" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1847" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2074" uniqueCount="88">
   <si>
     <t>index</t>
   </si>
@@ -283,6 +284,15 @@
   </si>
   <si>
     <t>value</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>voltage</t>
+  </si>
+  <si>
+    <t>220/380</t>
   </si>
 </sst>
 </file>
@@ -630,7 +640,7 @@
   <dimension ref="A1:AZ45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1065,6 +1075,15 @@
       </c>
     </row>
     <row r="6" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
+        <v>87</v>
+      </c>
       <c r="D6" t="s">
         <v>41</v>
       </c>
@@ -2060,7 +2079,7 @@
   <dimension ref="A1:BK23"/>
   <sheetViews>
     <sheetView topLeftCell="R1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="V20" sqref="V20"/>
+      <selection activeCell="Y1" sqref="Y1:AA6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4451,12 +4470,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="Y1:AA1"/>
-    <mergeCell ref="U1:W1"/>
-    <mergeCell ref="Q1:S1"/>
     <mergeCell ref="BI1:BK1"/>
     <mergeCell ref="AC1:AE1"/>
     <mergeCell ref="AG1:AI1"/>
@@ -4467,6 +4480,12 @@
     <mergeCell ref="AS1:AU1"/>
     <mergeCell ref="AW1:AY1"/>
     <mergeCell ref="BA1:BC1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="U1:W1"/>
+    <mergeCell ref="Q1:S1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4476,8 +4495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AY23"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AL10" sqref="AL10"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5341,6 +5360,15 @@
       </c>
     </row>
     <row r="9" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
       <c r="D9" t="s">
         <v>41</v>
       </c>
@@ -6494,12 +6522,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="U1:W1"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="Q1:S1"/>
     <mergeCell ref="AS1:AU1"/>
     <mergeCell ref="AW1:AY1"/>
     <mergeCell ref="Y1:AA1"/>
@@ -6507,6 +6529,12 @@
     <mergeCell ref="AG1:AI1"/>
     <mergeCell ref="AK1:AM1"/>
     <mergeCell ref="AO1:AQ1"/>
+    <mergeCell ref="U1:W1"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="Q1:S1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6517,7 +6545,7 @@
   <dimension ref="A1:T23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="B9" sqref="B9:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6891,6 +6919,15 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="b">
+        <v>0</v>
+      </c>
       <c r="D9" t="s">
         <v>41</v>
       </c>
@@ -6904,10 +6941,13 @@
         <v>41</v>
       </c>
       <c r="M9" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="N9" t="s">
-        <v>41</v>
+        <v>46</v>
+      </c>
+      <c r="O9" t="b">
+        <v>1</v>
       </c>
       <c r="T9" t="s">
         <v>41</v>
@@ -7251,4 +7291,850 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC335A7A-018D-4DAC-A385-A53EEC83747D}">
+  <dimension ref="A1:AA23"/>
+  <sheetViews>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="Z12" sqref="Z12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="I1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="M1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="Q1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="U1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="Y1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
+    </row>
+    <row r="2" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M3" t="s">
+        <v>0</v>
+      </c>
+      <c r="N3" t="s">
+        <v>45</v>
+      </c>
+      <c r="O3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>0</v>
+      </c>
+      <c r="R3" t="s">
+        <v>45</v>
+      </c>
+      <c r="S3" t="b">
+        <v>0</v>
+      </c>
+      <c r="U3" t="s">
+        <v>0</v>
+      </c>
+      <c r="V3" t="s">
+        <v>45</v>
+      </c>
+      <c r="W3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" t="s">
+        <v>47</v>
+      </c>
+      <c r="K4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" t="s">
+        <v>47</v>
+      </c>
+      <c r="O4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R4" t="s">
+        <v>45</v>
+      </c>
+      <c r="S4" t="b">
+        <v>0</v>
+      </c>
+      <c r="U4" t="s">
+        <v>29</v>
+      </c>
+      <c r="V4" t="s">
+        <v>45</v>
+      </c>
+      <c r="W4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J5" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5" t="b">
+        <v>0</v>
+      </c>
+      <c r="M5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" t="s">
+        <v>47</v>
+      </c>
+      <c r="O5" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>8</v>
+      </c>
+      <c r="R5" t="s">
+        <v>47</v>
+      </c>
+      <c r="S5" t="b">
+        <v>0</v>
+      </c>
+      <c r="U5" t="s">
+        <v>67</v>
+      </c>
+      <c r="V5" t="s">
+        <v>69</v>
+      </c>
+      <c r="W5" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" t="b">
+        <v>0</v>
+      </c>
+      <c r="M6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N6" t="s">
+        <v>46</v>
+      </c>
+      <c r="O6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>43</v>
+      </c>
+      <c r="R6" t="s">
+        <v>21</v>
+      </c>
+      <c r="S6" t="b">
+        <v>0</v>
+      </c>
+      <c r="U6" t="s">
+        <v>16</v>
+      </c>
+      <c r="V6" t="s">
+        <v>46</v>
+      </c>
+      <c r="W6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J7" t="s">
+        <v>45</v>
+      </c>
+      <c r="K7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M7" t="s">
+        <v>85</v>
+      </c>
+      <c r="N7" t="s">
+        <v>46</v>
+      </c>
+      <c r="O7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" t="s">
+        <v>45</v>
+      </c>
+      <c r="K8" t="b">
+        <v>0</v>
+      </c>
+      <c r="M8" t="s">
+        <v>15</v>
+      </c>
+      <c r="N8" t="s">
+        <v>46</v>
+      </c>
+      <c r="O8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" t="s">
+        <v>41</v>
+      </c>
+      <c r="M9" t="s">
+        <v>54</v>
+      </c>
+      <c r="N9" t="s">
+        <v>6</v>
+      </c>
+      <c r="O9" t="b">
+        <v>0</v>
+      </c>
+      <c r="T9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" t="s">
+        <v>41</v>
+      </c>
+      <c r="N10" t="s">
+        <v>41</v>
+      </c>
+      <c r="T10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" t="s">
+        <v>41</v>
+      </c>
+      <c r="N11" t="s">
+        <v>41</v>
+      </c>
+      <c r="T11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" t="s">
+        <v>41</v>
+      </c>
+      <c r="N12" t="s">
+        <v>41</v>
+      </c>
+      <c r="T12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" t="s">
+        <v>41</v>
+      </c>
+      <c r="M13" t="s">
+        <v>41</v>
+      </c>
+      <c r="N13" t="s">
+        <v>41</v>
+      </c>
+      <c r="T13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" t="s">
+        <v>41</v>
+      </c>
+      <c r="M14" t="s">
+        <v>41</v>
+      </c>
+      <c r="N14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" t="s">
+        <v>41</v>
+      </c>
+      <c r="M15" t="s">
+        <v>41</v>
+      </c>
+      <c r="N15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" t="s">
+        <v>41</v>
+      </c>
+      <c r="M16" t="s">
+        <v>41</v>
+      </c>
+      <c r="N16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="4:20" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17" t="s">
+        <v>41</v>
+      </c>
+      <c r="M17" t="s">
+        <v>41</v>
+      </c>
+      <c r="N17" t="s">
+        <v>41</v>
+      </c>
+      <c r="R17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="4:20" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" t="s">
+        <v>41</v>
+      </c>
+      <c r="M18" t="s">
+        <v>41</v>
+      </c>
+      <c r="N18" t="s">
+        <v>41</v>
+      </c>
+      <c r="R18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="4:20" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" t="s">
+        <v>41</v>
+      </c>
+      <c r="M19" t="s">
+        <v>41</v>
+      </c>
+      <c r="N19" t="s">
+        <v>41</v>
+      </c>
+      <c r="P19" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>41</v>
+      </c>
+      <c r="R19" t="s">
+        <v>41</v>
+      </c>
+      <c r="T19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="4:20" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" t="s">
+        <v>41</v>
+      </c>
+      <c r="M20" t="s">
+        <v>41</v>
+      </c>
+      <c r="N20" t="s">
+        <v>41</v>
+      </c>
+      <c r="P20" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>41</v>
+      </c>
+      <c r="R20" t="s">
+        <v>41</v>
+      </c>
+      <c r="T20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="4:20" x14ac:dyDescent="0.3">
+      <c r="D21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" t="s">
+        <v>41</v>
+      </c>
+      <c r="G21" t="s">
+        <v>41</v>
+      </c>
+      <c r="M21" t="s">
+        <v>41</v>
+      </c>
+      <c r="N21" t="s">
+        <v>41</v>
+      </c>
+      <c r="P21" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>41</v>
+      </c>
+      <c r="R21" t="s">
+        <v>41</v>
+      </c>
+      <c r="T21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="4:20" x14ac:dyDescent="0.3">
+      <c r="D22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" t="s">
+        <v>41</v>
+      </c>
+      <c r="G22" t="s">
+        <v>41</v>
+      </c>
+      <c r="M22" t="s">
+        <v>41</v>
+      </c>
+      <c r="N22" t="s">
+        <v>41</v>
+      </c>
+      <c r="T22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="4:20" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" t="s">
+        <v>41</v>
+      </c>
+      <c r="G23" t="s">
+        <v>41</v>
+      </c>
+      <c r="M23" t="s">
+        <v>41</v>
+      </c>
+      <c r="N23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="U1:W1"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="Q1:S1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
matpower casedata, transformer identification
</commit_message>
<xml_diff>
--- a/examples/data_input/data_structure.xlsx
+++ b/examples/data_input/data_structure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riw\tubCloud\Uni\Market_Tool\pomato_studies\data_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{392C7022-03AC-472B-83F6-72FAC9E760B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9084BA-0F64-4B5A-A526-CEDFB3348659}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="948" yWindow="0" windowWidth="26892" windowHeight="17280" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1224" yWindow="-108" windowWidth="40164" windowHeight="17496" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="7" r:id="rId1"/>
@@ -19,17 +19,25 @@
     <sheet name="ieee" sheetId="6" r:id="rId4"/>
     <sheet name="nrel" sheetId="9" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2074" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2056" uniqueCount="88">
   <si>
     <t>index</t>
   </si>
@@ -292,7 +300,7 @@
     <t>voltage</t>
   </si>
   <si>
-    <t>220/380</t>
+    <t>technology</t>
   </si>
 </sst>
 </file>
@@ -640,7 +648,7 @@
   <dimension ref="A1:AZ45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1081,8 +1089,8 @@
       <c r="B6" t="s">
         <v>46</v>
       </c>
-      <c r="C6" t="s">
-        <v>87</v>
+      <c r="C6">
+        <v>220</v>
       </c>
       <c r="D6" t="s">
         <v>41</v>
@@ -2078,8 +2086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BK23"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Y1" sqref="Y1:AA6"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AI28" sqref="AI28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3019,13 +3027,13 @@
     </row>
     <row r="8" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>86</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" t="s">
         <v>41</v>
@@ -3057,23 +3065,20 @@
       <c r="O8" t="b">
         <v>0</v>
       </c>
-      <c r="Q8" t="s">
-        <v>59</v>
-      </c>
-      <c r="R8" t="s">
-        <v>46</v>
-      </c>
-      <c r="S8" t="b">
+      <c r="U8" t="s">
+        <v>60</v>
+      </c>
+      <c r="V8" t="s">
+        <v>46</v>
+      </c>
+      <c r="W8" t="b">
         <v>1</v>
       </c>
-      <c r="U8" t="s">
-        <v>28</v>
-      </c>
-      <c r="V8" t="s">
-        <v>46</v>
-      </c>
-      <c r="W8" t="b">
-        <v>0</v>
+      <c r="Y8" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>41</v>
       </c>
       <c r="AA8" t="s">
         <v>41</v>
@@ -3088,7 +3093,7 @@
         <v>0</v>
       </c>
       <c r="AG8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AH8" t="s">
         <v>45</v>
@@ -3096,6 +3101,21 @@
       <c r="AI8" t="b">
         <v>1</v>
       </c>
+      <c r="AK8" t="s">
+        <v>41</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM8" t="s">
+        <v>41</v>
+      </c>
+      <c r="AO8" t="s">
+        <v>41</v>
+      </c>
+      <c r="AP8" t="s">
+        <v>41</v>
+      </c>
       <c r="AQ8" t="s">
         <v>41</v>
       </c>
@@ -3108,8 +3128,23 @@
       <c r="AU8" t="s">
         <v>41</v>
       </c>
+      <c r="AY8" t="s">
+        <v>41</v>
+      </c>
+      <c r="BA8" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="9" spans="1:63" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
       <c r="D9" t="s">
         <v>41</v>
       </c>
@@ -3141,7 +3176,7 @@
         <v>0</v>
       </c>
       <c r="U9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="V9" t="s">
         <v>46</v>
@@ -3149,12 +3184,6 @@
       <c r="W9" t="b">
         <v>1</v>
       </c>
-      <c r="Y9" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>41</v>
-      </c>
       <c r="AA9" t="s">
         <v>41</v>
       </c>
@@ -3168,10 +3197,10 @@
         <v>1</v>
       </c>
       <c r="AG9" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="AH9" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="AI9" t="b">
         <v>1</v>
@@ -3211,27 +3240,6 @@
       </c>
     </row>
     <row r="10" spans="1:63" x14ac:dyDescent="0.3">
-      <c r="D10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" t="s">
-        <v>41</v>
-      </c>
-      <c r="I10" t="s">
-        <v>41</v>
-      </c>
-      <c r="J10" t="s">
-        <v>41</v>
-      </c>
-      <c r="K10" t="s">
-        <v>41</v>
-      </c>
       <c r="M10" t="s">
         <v>11</v>
       </c>
@@ -3242,7 +3250,7 @@
         <v>0</v>
       </c>
       <c r="U10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="V10" t="s">
         <v>46</v>
@@ -3250,9 +3258,6 @@
       <c r="W10" t="b">
         <v>1</v>
       </c>
-      <c r="AA10" t="s">
-        <v>41</v>
-      </c>
       <c r="AC10" t="s">
         <v>32</v>
       </c>
@@ -3263,7 +3268,7 @@
         <v>1</v>
       </c>
       <c r="AG10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AH10" t="s">
         <v>49</v>
@@ -3271,39 +3276,6 @@
       <c r="AI10" t="b">
         <v>1</v>
       </c>
-      <c r="AK10" t="s">
-        <v>41</v>
-      </c>
-      <c r="AL10" t="s">
-        <v>41</v>
-      </c>
-      <c r="AM10" t="s">
-        <v>41</v>
-      </c>
-      <c r="AO10" t="s">
-        <v>41</v>
-      </c>
-      <c r="AP10" t="s">
-        <v>41</v>
-      </c>
-      <c r="AQ10" t="s">
-        <v>41</v>
-      </c>
-      <c r="AS10" t="s">
-        <v>41</v>
-      </c>
-      <c r="AT10" t="s">
-        <v>41</v>
-      </c>
-      <c r="AU10" t="s">
-        <v>41</v>
-      </c>
-      <c r="AY10" t="s">
-        <v>41</v>
-      </c>
-      <c r="BA10" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="11" spans="1:63" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
@@ -3337,7 +3309,7 @@
         <v>0</v>
       </c>
       <c r="U11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="V11" t="s">
         <v>46</v>
@@ -3358,10 +3330,10 @@
         <v>1</v>
       </c>
       <c r="AG11" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="AH11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="AI11" t="b">
         <v>1</v>
@@ -3438,7 +3410,7 @@
         <v>0</v>
       </c>
       <c r="U12" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="V12" t="s">
         <v>46</v>
@@ -3458,15 +3430,6 @@
       <c r="AE12" t="b">
         <v>1</v>
       </c>
-      <c r="AG12" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH12" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI12" t="b">
-        <v>1</v>
-      </c>
       <c r="AK12" t="s">
         <v>41</v>
       </c>
@@ -3538,15 +3501,6 @@
       <c r="O13" t="b">
         <v>1</v>
       </c>
-      <c r="U13" t="s">
-        <v>59</v>
-      </c>
-      <c r="V13" t="s">
-        <v>46</v>
-      </c>
-      <c r="W13" t="b">
-        <v>1</v>
-      </c>
       <c r="Y13" t="s">
         <v>41</v>
       </c>
@@ -3915,11 +3869,14 @@
       <c r="AA17" t="s">
         <v>41</v>
       </c>
+      <c r="AC17" t="s">
+        <v>87</v>
+      </c>
       <c r="AD17" t="s">
-        <v>41</v>
-      </c>
-      <c r="AE17" t="s">
-        <v>41</v>
+        <v>45</v>
+      </c>
+      <c r="AE17" t="b">
+        <v>1</v>
       </c>
       <c r="AF17" t="s">
         <v>41</v>
@@ -4470,6 +4427,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="U1:W1"/>
+    <mergeCell ref="Q1:S1"/>
     <mergeCell ref="BI1:BK1"/>
     <mergeCell ref="AC1:AE1"/>
     <mergeCell ref="AG1:AI1"/>
@@ -4480,12 +4443,6 @@
     <mergeCell ref="AS1:AU1"/>
     <mergeCell ref="AW1:AY1"/>
     <mergeCell ref="BA1:BC1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="Y1:AA1"/>
-    <mergeCell ref="U1:W1"/>
-    <mergeCell ref="Q1:S1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4496,7 +4453,7 @@
   <dimension ref="A1:AY23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="V34" sqref="V34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5637,7 +5594,7 @@
         <v>41</v>
       </c>
       <c r="AC12" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="AD12" t="s">
         <v>46</v>
@@ -5950,12 +5907,6 @@
       <c r="AA16" t="s">
         <v>41</v>
       </c>
-      <c r="AD16" t="s">
-        <v>41</v>
-      </c>
-      <c r="AE16" t="s">
-        <v>41</v>
-      </c>
       <c r="AG16" t="s">
         <v>41</v>
       </c>
@@ -6522,6 +6473,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="U1:W1"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="Q1:S1"/>
     <mergeCell ref="AS1:AU1"/>
     <mergeCell ref="AW1:AY1"/>
     <mergeCell ref="Y1:AA1"/>
@@ -6529,12 +6486,6 @@
     <mergeCell ref="AG1:AI1"/>
     <mergeCell ref="AK1:AM1"/>
     <mergeCell ref="AO1:AQ1"/>
-    <mergeCell ref="U1:W1"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="Q1:S1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6545,7 +6496,7 @@
   <dimension ref="A1:T23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:C9"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6941,7 +6892,7 @@
         <v>41</v>
       </c>
       <c r="M9" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="N9" t="s">
         <v>46</v>
@@ -6966,8 +6917,14 @@
       <c r="G10" t="s">
         <v>41</v>
       </c>
+      <c r="M10" t="s">
+        <v>34</v>
+      </c>
       <c r="N10" t="s">
-        <v>41</v>
+        <v>46</v>
+      </c>
+      <c r="O10" t="b">
+        <v>1</v>
       </c>
       <c r="T10" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
remove MarketModel and RedundancyRemoval to seperate repositories. Installation process mostly unchanged, but better
</commit_message>
<xml_diff>
--- a/examples/data_input/data_structure.xlsx
+++ b/examples/data_input/data_structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riw\tubCloud\Uni\Market_Tool\pomato_studies\data_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9084BA-0F64-4B5A-A526-CEDFB3348659}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3CA555E-DDFD-4D4B-9454-E002FB59F12E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1224" yWindow="-108" windowWidth="40164" windowHeight="17496" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1476" yWindow="0" windowWidth="34788" windowHeight="17280" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="7" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2056" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2060" uniqueCount="89">
   <si>
     <t>index</t>
   </si>
@@ -301,6 +301,9 @@
   </si>
   <si>
     <t>technology</t>
+  </si>
+  <si>
+    <t>r</t>
   </si>
 </sst>
 </file>
@@ -648,7 +651,7 @@
   <dimension ref="A1:AZ45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4427,12 +4430,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="Y1:AA1"/>
-    <mergeCell ref="U1:W1"/>
-    <mergeCell ref="Q1:S1"/>
     <mergeCell ref="BI1:BK1"/>
     <mergeCell ref="AC1:AE1"/>
     <mergeCell ref="AG1:AI1"/>
@@ -4443,6 +4440,12 @@
     <mergeCell ref="AS1:AU1"/>
     <mergeCell ref="AW1:AY1"/>
     <mergeCell ref="BA1:BC1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="U1:W1"/>
+    <mergeCell ref="Q1:S1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6473,12 +6476,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="U1:W1"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="Q1:S1"/>
     <mergeCell ref="AS1:AU1"/>
     <mergeCell ref="AW1:AY1"/>
     <mergeCell ref="Y1:AA1"/>
@@ -6486,6 +6483,12 @@
     <mergeCell ref="AG1:AI1"/>
     <mergeCell ref="AK1:AM1"/>
     <mergeCell ref="AO1:AQ1"/>
+    <mergeCell ref="U1:W1"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="Q1:S1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6496,7 +6499,7 @@
   <dimension ref="A1:T23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6943,8 +6946,14 @@
       <c r="G11" t="s">
         <v>41</v>
       </c>
+      <c r="M11" t="s">
+        <v>86</v>
+      </c>
       <c r="N11" t="s">
-        <v>41</v>
+        <v>45</v>
+      </c>
+      <c r="O11" t="b">
+        <v>1</v>
       </c>
       <c r="T11" t="s">
         <v>41</v>
@@ -7255,7 +7264,7 @@
   <dimension ref="A1:AA23"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Z12" sqref="Z12"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7719,7 +7728,7 @@
         <v>0</v>
       </c>
       <c r="M8" t="s">
-        <v>15</v>
+        <v>88</v>
       </c>
       <c r="N8" t="s">
         <v>46</v>
@@ -7742,10 +7751,10 @@
         <v>41</v>
       </c>
       <c r="M9" t="s">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="N9" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="O9" t="b">
         <v>0</v>
@@ -7767,8 +7776,14 @@
       <c r="G10" t="s">
         <v>41</v>
       </c>
+      <c r="M10" t="s">
+        <v>54</v>
+      </c>
       <c r="N10" t="s">
-        <v>41</v>
+        <v>6</v>
+      </c>
+      <c r="O10" t="b">
+        <v>0</v>
       </c>
       <c r="T10" t="s">
         <v>41</v>
@@ -7787,8 +7802,14 @@
       <c r="G11" t="s">
         <v>41</v>
       </c>
+      <c r="M11" t="s">
+        <v>86</v>
+      </c>
       <c r="N11" t="s">
-        <v>41</v>
+        <v>45</v>
+      </c>
+      <c r="O11" t="b">
+        <v>1</v>
       </c>
       <c r="T11" t="s">
         <v>41</v>
@@ -7807,8 +7828,14 @@
       <c r="G12" t="s">
         <v>41</v>
       </c>
+      <c r="M12" t="s">
+        <v>87</v>
+      </c>
       <c r="N12" t="s">
-        <v>41</v>
+        <v>45</v>
+      </c>
+      <c r="O12" t="b">
+        <v>1</v>
       </c>
       <c r="T12" t="s">
         <v>41</v>

</xml_diff>